<commit_message>
Gantt + maj journal
</commit_message>
<xml_diff>
--- a/Semaine 11/Journal de travail - Dylan Metral.xlsx
+++ b/Semaine 11/Journal de travail - Dylan Metral.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Tâche effectuées</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Création de la partie 3</t>
+  </si>
+  <si>
+    <t>Mise à jour du Gantt</t>
   </si>
 </sst>
 </file>
@@ -191,14 +194,26 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -207,20 +222,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,10 +532,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:G37"/>
+  <dimension ref="B3:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:G33"/>
+      <selection activeCell="D36" sqref="D36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,14 +545,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -562,58 +565,58 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -626,24 +629,24 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -656,24 +659,24 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
@@ -686,24 +689,24 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
@@ -716,44 +719,44 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -766,24 +769,24 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
@@ -796,24 +799,24 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="2"/>
+      <c r="D28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="4"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -826,24 +829,24 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="8" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="4"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
@@ -856,47 +859,114 @@
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="8" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="4"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="53">
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:C40"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="F39:G40"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="D17:E18"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="D22:E23"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="D36:E37"/>
@@ -913,39 +983,6 @@
     <mergeCell ref="F25:G26"/>
     <mergeCell ref="F28:G29"/>
     <mergeCell ref="D28:E29"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="D17:E18"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="D25:E26"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="D14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>